<commit_message>
xoa va tao course
</commit_message>
<xml_diff>
--- a/public/resource/xlsx/l.xlsx
+++ b/public/resource/xlsx/l.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,39 +19,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Lê Đình Thanh</t>
-  </si>
-  <si>
-    <t>thanhld</t>
-  </si>
-  <si>
-    <t>tunghx</t>
-  </si>
-  <si>
-    <t>sonnh</t>
-  </si>
-  <si>
-    <t>thudm</t>
-  </si>
-  <si>
-    <t>maitt</t>
-  </si>
-  <si>
-    <t> Hoàng Xuân Tùng</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoài Sơn</t>
-  </si>
-  <si>
-    <t>Đào Minh Thư</t>
-  </si>
-  <si>
-    <t>Trần Trúc Mai</t>
+    <t> 15020881</t>
+  </si>
+  <si>
+    <t> Triệu Hoàng An</t>
+  </si>
+  <si>
+    <t> 15021394</t>
+  </si>
+  <si>
+    <t> Bùi Châu Anh</t>
+  </si>
+  <si>
+    <t> Lưu Việt Anh</t>
+  </si>
+  <si>
+    <t> 15021976</t>
+  </si>
+  <si>
+    <t> Nguyễn Đức Anh</t>
+  </si>
+  <si>
+    <t> 15021483</t>
+  </si>
+  <si>
+    <t> Nguyễn Quang Anh</t>
+  </si>
+  <si>
+    <t> 15022841</t>
+  </si>
+  <si>
+    <t> Nguyễn Thị Phương Anh</t>
+  </si>
+  <si>
+    <t> 15021332</t>
+  </si>
+  <si>
+    <t> Nguyễn Thị Vân Anh</t>
+  </si>
+  <si>
+    <t> 15021849</t>
+  </si>
+  <si>
+    <t> Nguyễn Tuấn Anh</t>
+  </si>
+  <si>
+    <t> 15021469</t>
+  </si>
+  <si>
+    <t> Nguyễn Chu Chiến</t>
+  </si>
+  <si>
+    <t> 15021359</t>
+  </si>
+  <si>
+    <t> Trần Minh Chiến</t>
+  </si>
+  <si>
+    <t>QH-2015-I/CQ-CLC</t>
   </si>
   <si>
     <t>username</t>
@@ -64,6 +94,9 @@
   </si>
   <si>
     <t>vnuemail</t>
+  </si>
+  <si>
+    <t>classname</t>
   </si>
 </sst>
 </file>
@@ -457,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,47 +503,54 @@
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" customWidth="1"/>
-    <col min="42" max="42" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="20" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" customWidth="1"/>
+    <col min="43" max="43" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>12345678</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" ref="E2:E6" si="0">B2&amp;"@vnu.edu.vn"</f>
-        <v>thanhld@vnu.edu.vn</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="E2:E11" si="0">B2&amp;"@vnu.edu.vn"</f>
+        <v> 15020881@vnu.edu.vn</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -521,81 +561,701 @@
         <v>12345678</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>tunghx@vnu.edu.vn</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v> 15021394@vnu.edu.vn</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
+      <c r="B4" s="4">
+        <v>15021606</v>
       </c>
       <c r="C4" s="2">
         <v>12345678</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>sonnh@vnu.edu.vn</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>B4&amp;"@vnu.edu.vn"</f>
+        <v>15021606@vnu.edu.vn</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>12345678</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>thudm@vnu.edu.vn</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v> 15021976@vnu.edu.vn</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>12345678</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>maitt@vnu.edu.vn</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+        <v> 15021483@vnu.edu.vn</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f>B7&amp;"@vnu.edu.vn"</f>
+        <v> 15022841@vnu.edu.vn</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v> 15021332@vnu.edu.vn</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v> 15021849@vnu.edu.vn</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v> 15021469@vnu.edu.vn</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v> 15021359@vnu.edu.vn</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="dungnd_58@vnu.edu.vn"/>
-    <hyperlink ref="E3:E6" r:id="rId2" display="dungnd_58@vnu.edu.vn"/>
+    <hyperlink ref="E3:E8" r:id="rId2" display="dungnd_58@vnu.edu.vn"/>
+    <hyperlink ref="E9" r:id="rId3" display="dungnd_58@vnu.edu.vn"/>
+    <hyperlink ref="E10:E11" r:id="rId4" display="dungnd_58@vnu.edu.vn"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>